<commit_message>
we have updated the time out and modified the code to show message
</commit_message>
<xml_diff>
--- a/UtilityFolder/TutorialsNinja.xlsx
+++ b/UtilityFolder/TutorialsNinja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harshavardhan\eclipse-workspace\DataDrivenFrameworkProject\UtilityFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C7F42B-1767-421A-B2E9-B007DB6D9BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138EA6C7-736D-4A79-936F-683515251518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{69BD690B-6A4F-48D2-BFF0-BB443C6E980C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>TestCase</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Firefox</t>
   </si>
   <si>
-    <t>amotooricap1@gmail.com</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Harsh@9334</t>
+  </si>
+  <si>
+    <t>harshvardhan9661@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -691,7 +691,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -742,10 +742,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
@@ -755,7 +755,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -763,13 +763,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="11">
-        <v>12345</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -781,16 +781,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="11">
         <v>12345</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -829,22 +829,22 @@
         <v>7</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="E8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>10</v>
@@ -858,13 +858,13 @@
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="F9" s="12">
         <v>1234567890</v>
@@ -876,7 +876,7 @@
         <v>12345</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -887,13 +887,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12">
         <v>1234567891</v>
@@ -905,7 +905,7 @@
         <v>12345</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -916,13 +916,13 @@
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="12">
         <v>1234567892</v>
@@ -934,7 +934,7 @@
         <v>12345</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -945,13 +945,13 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="12">
         <v>1234567893</v>
@@ -963,7 +963,7 @@
         <v>12345</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -990,10 +990,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="mailto:amotooricap1@gmail.com" xr:uid="{08F4FFFE-4864-4512-8E7A-A08DB06C2435}"/>
-    <hyperlink ref="C5" r:id="rId2" display="mailto:amotooricap3@gmail.com" xr:uid="{C8FE460B-26AF-4265-831A-13F760B1467E}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{B79BDB27-C409-4B3D-BB0E-616FFDBEC8E6}"/>
-    <hyperlink ref="D3" r:id="rId4" xr:uid="{ACD92B29-D947-4160-8D2A-5D4667A40AA7}"/>
+    <hyperlink ref="C5" r:id="rId1" display="mailto:amotooricap3@gmail.com" xr:uid="{C8FE460B-26AF-4265-831A-13F760B1467E}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{B79BDB27-C409-4B3D-BB0E-616FFDBEC8E6}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{ACD92B29-D947-4160-8D2A-5D4667A40AA7}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{587A9BE5-6E41-4803-83EC-6FDCC488A509}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{F0D71886-D9DF-4879-BF4B-0FBC48F68828}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>